<commit_message>
started implementing giga center
</commit_message>
<xml_diff>
--- a/preprocessing/MFMS_Daten.xlsx
+++ b/preprocessing/MFMS_Daten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theresawettig/superblock/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35490A76-94B6-9C4F-AB67-9EB16C2932F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E553F4E2-24A7-504C-BF76-1E1FA72EDEA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4280" yWindow="460" windowWidth="20660" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -46,14 +46,41 @@
         <r>
           <rPr>
             <sz val="11"/>
-            <color theme="1"/>
+            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>======
-ID#AAAAGs6FkF0
-Julia    (2020-07-11 09:55:30)
-BKA: 90,229 Straftaten im Jahr in München; 90,229 / 365 = 247 pro Tag</t>
+          <t xml:space="preserve">======
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">ID#AAAAGs6FkF0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Julia    (2020-07-11 09:55:30)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>BKA: 90,229 Straftaten im Jahr in München; 90,229 / 365 = 247 pro Tag</t>
         </r>
       </text>
     </comment>
@@ -67,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="82">
   <si>
     <t>Center Typ</t>
   </si>
@@ -304,6 +331,15 @@
   </si>
   <si>
     <t>demand_rate_c</t>
+  </si>
+  <si>
+    <t>GC?</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
   </si>
 </sst>
 </file>
@@ -314,7 +350,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,12 +444,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -735,7 +765,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -770,6 +800,9 @@
       <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="H1" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
@@ -789,6 +822,9 @@
       <c r="G2" s="8">
         <v>10</v>
       </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
@@ -808,6 +844,9 @@
       <c r="G3" s="8">
         <v>468</v>
       </c>
+      <c r="H3" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
@@ -827,6 +866,9 @@
       <c r="G4" s="8">
         <v>6</v>
       </c>
+      <c r="H4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
@@ -846,6 +888,9 @@
       <c r="G5" s="8">
         <v>9</v>
       </c>
+      <c r="H5" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
@@ -867,6 +912,9 @@
         <v>70</v>
       </c>
       <c r="G6" s="13"/>
+      <c r="H6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
@@ -888,6 +936,9 @@
         <v>20</v>
       </c>
       <c r="G7" s="13"/>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
@@ -909,6 +960,9 @@
         <v>50</v>
       </c>
       <c r="G8" s="13"/>
+      <c r="H8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
@@ -930,6 +984,9 @@
         <v>4</v>
       </c>
       <c r="G9" s="13"/>
+      <c r="H9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="16" t="s">
@@ -948,6 +1005,9 @@
       <c r="G10" s="19">
         <v>25</v>
       </c>
+      <c r="H10" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16" t="s">
@@ -965,6 +1025,9 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="20"/>
+      <c r="H11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
@@ -976,6 +1039,9 @@
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="21"/>
+      <c r="H12" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
@@ -987,6 +1053,9 @@
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="21"/>
+      <c r="H13" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="16" t="s">
@@ -1006,6 +1075,9 @@
       <c r="G14" s="19">
         <v>10</v>
       </c>
+      <c r="H14" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="22" t="s">
@@ -1025,6 +1097,9 @@
       </c>
       <c r="F15" s="24"/>
       <c r="G15" s="25"/>
+      <c r="H15" t="s">
+        <v>80</v>
+      </c>
       <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1047,6 +1122,9 @@
       <c r="G16" s="27">
         <v>4</v>
       </c>
+      <c r="H16" t="s">
+        <v>81</v>
+      </c>
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1071,6 +1149,9 @@
       <c r="G17" s="24">
         <v>5</v>
       </c>
+      <c r="H17" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="I17" s="28"/>
     </row>
     <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1095,6 +1176,9 @@
       <c r="G18" s="24">
         <v>2</v>
       </c>
+      <c r="H18" s="24" t="s">
+        <v>81</v>
+      </c>
       <c r="I18" s="28"/>
     </row>
     <row r="19" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -1117,6 +1201,9 @@
         <v>34</v>
       </c>
       <c r="G19" s="18"/>
+      <c r="H19" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="21" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
use ob sets + subsets
</commit_message>
<xml_diff>
--- a/preprocessing/MFMS_Daten.xlsx
+++ b/preprocessing/MFMS_Daten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theresawettig/superblock/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E553F4E2-24A7-504C-BF76-1E1FA72EDEA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD2FC2F-E884-F043-89DA-1FC3838334F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4280" yWindow="460" windowWidth="20660" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -765,7 +765,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>